<commit_message>
monthwise sheet function added
</commit_message>
<xml_diff>
--- a/PU32.xlsx
+++ b/PU32.xlsx
@@ -620,9 +620,9 @@
           <t>Expenditure Under</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>PU32</t>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Fig in crore</t>
         </is>
       </c>
     </row>
@@ -677,21 +677,29 @@
     </row>
     <row r="3" ht="15.75" customFormat="1" customHeight="1" s="1" thickBot="1">
       <c r="A3" s="20" t="n"/>
-      <c r="B3" s="10" t="n"/>
-      <c r="C3" s="10" t="n"/>
+      <c r="B3" s="10" t="inlineStr">
+        <is>
+          <t>2021-22</t>
+        </is>
+      </c>
+      <c r="C3" s="10" t="inlineStr">
+        <is>
+          <t>2022-23</t>
+        </is>
+      </c>
       <c r="D3" s="10" t="inlineStr">
         <is>
-          <t>JAN' 21</t>
+          <t>JUN' 21</t>
         </is>
       </c>
       <c r="E3" s="10" t="inlineStr">
         <is>
-          <t>JAN' 22</t>
+          <t>JUN' 22</t>
         </is>
       </c>
       <c r="F3" s="8" t="inlineStr">
         <is>
-          <t>JAN' 22</t>
+          <t>JUN' 22</t>
         </is>
       </c>
       <c r="G3" s="12" t="inlineStr">
@@ -726,18 +734,20 @@
           <t>SMH 01 (D-03)</t>
         </is>
       </c>
-      <c r="B4" s="16" t="n"/>
+      <c r="B4" s="16" t="n">
+        <v>7.72</v>
+      </c>
       <c r="C4" s="16" t="n">
-        <v>6.7</v>
+        <v>6.29</v>
       </c>
       <c r="D4" s="16" t="n">
-        <v>6.11</v>
+        <v>1.58</v>
       </c>
       <c r="E4" s="16" t="n">
-        <v>5.87</v>
+        <v>1.64</v>
       </c>
       <c r="F4" s="16" t="n">
-        <v>6.33</v>
+        <v>2.7</v>
       </c>
       <c r="G4" s="16">
         <f>F4-E4</f>
@@ -766,18 +776,20 @@
           <t>SMH 02 (D-04)</t>
         </is>
       </c>
-      <c r="B5" s="11" t="n"/>
+      <c r="B5" s="11" t="n">
+        <v>90.73</v>
+      </c>
       <c r="C5" s="11" t="n">
-        <v>84.51000000000001</v>
+        <v>79.2</v>
       </c>
       <c r="D5" s="11" t="n">
-        <v>92.22</v>
+        <v>21.18</v>
       </c>
       <c r="E5" s="11" t="n">
-        <v>71.06</v>
+        <v>20.59</v>
       </c>
       <c r="F5" s="11" t="n">
-        <v>76.5</v>
+        <v>29.56</v>
       </c>
       <c r="G5" s="11">
         <f>F5-E5</f>
@@ -806,18 +818,20 @@
           <t>SMH 03 (D-05)</t>
         </is>
       </c>
-      <c r="B6" s="11" t="n"/>
+      <c r="B6" s="11" t="n">
+        <v>11.38</v>
+      </c>
       <c r="C6" s="11" t="n">
-        <v>9.619999999999999</v>
+        <v>9.039999999999999</v>
       </c>
       <c r="D6" s="11" t="n">
-        <v>9.16</v>
+        <v>0.7</v>
       </c>
       <c r="E6" s="11" t="n">
-        <v>8.390000000000001</v>
+        <v>2.35</v>
       </c>
       <c r="F6" s="11" t="n">
-        <v>9.140000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="G6" s="11">
         <f>F6-E6</f>
@@ -846,18 +860,20 @@
           <t>SMH 04 (D-06)</t>
         </is>
       </c>
-      <c r="B7" s="11" t="n"/>
+      <c r="B7" s="11" t="n">
+        <v>12.51</v>
+      </c>
       <c r="C7" s="11" t="n">
-        <v>12.42</v>
+        <v>11.67</v>
       </c>
       <c r="D7" s="11" t="n">
-        <v>10.93</v>
+        <v>2.79</v>
       </c>
       <c r="E7" s="11" t="n">
-        <v>10.44</v>
+        <v>3.03</v>
       </c>
       <c r="F7" s="11" t="n">
-        <v>11.22</v>
+        <v>3.02</v>
       </c>
       <c r="G7" s="11">
         <f>F7-E7</f>
@@ -886,18 +902,20 @@
           <t>SMH 05(D-07)</t>
         </is>
       </c>
-      <c r="B8" s="11" t="n"/>
+      <c r="B8" s="11" t="n">
+        <v>75.31</v>
+      </c>
       <c r="C8" s="11" t="n">
-        <v>72.55</v>
+        <v>68.11</v>
       </c>
       <c r="D8" s="11" t="n">
-        <v>55.45</v>
+        <v>20.45</v>
       </c>
       <c r="E8" s="11" t="n">
-        <v>56.51</v>
+        <v>17.71</v>
       </c>
       <c r="F8" s="11" t="n">
-        <v>63.33</v>
+        <v>18.74</v>
       </c>
       <c r="G8" s="11">
         <f>F8-E8</f>
@@ -926,18 +944,20 @@
           <t>SMH 06(D-08)</t>
         </is>
       </c>
-      <c r="B9" s="11" t="n"/>
+      <c r="B9" s="11" t="n">
+        <v>68.48</v>
+      </c>
       <c r="C9" s="11" t="n">
-        <v>57.4</v>
+        <v>53.89</v>
       </c>
       <c r="D9" s="11" t="n">
-        <v>43.81</v>
+        <v>13.66</v>
       </c>
       <c r="E9" s="11" t="n">
-        <v>42.8</v>
+        <v>14.01</v>
       </c>
       <c r="F9" s="11" t="n">
-        <v>53.9</v>
+        <v>17.39</v>
       </c>
       <c r="G9" s="11">
         <f>F9-E9</f>
@@ -966,18 +986,20 @@
           <t>SMH 07(D-09)</t>
         </is>
       </c>
-      <c r="B10" s="11" t="n"/>
+      <c r="B10" s="11" t="n">
+        <v>37.83</v>
+      </c>
       <c r="C10" s="11" t="n">
-        <v>32.41</v>
+        <v>30.43</v>
       </c>
       <c r="D10" s="11" t="n">
-        <v>37.21</v>
+        <v>7.8</v>
       </c>
       <c r="E10" s="11" t="n">
-        <v>30.82</v>
+        <v>7.91</v>
       </c>
       <c r="F10" s="11" t="n">
-        <v>30.62</v>
+        <v>12.12</v>
       </c>
       <c r="G10" s="11">
         <f>F10-E10</f>
@@ -1006,7 +1028,9 @@
           <t>SMH 08(D-10)</t>
         </is>
       </c>
-      <c r="B11" s="11" t="n"/>
+      <c r="B11" s="11" t="n">
+        <v>0</v>
+      </c>
       <c r="C11" s="11" t="n">
         <v>0</v>
       </c>
@@ -1046,18 +1070,20 @@
           <t>SMH 09(D-11)</t>
         </is>
       </c>
-      <c r="B12" s="11" t="n"/>
+      <c r="B12" s="11" t="n">
+        <v>37.84</v>
+      </c>
       <c r="C12" s="11" t="n">
-        <v>34.46</v>
+        <v>32.36</v>
       </c>
       <c r="D12" s="11" t="n">
-        <v>35.1</v>
+        <v>8.890000000000001</v>
       </c>
       <c r="E12" s="11" t="n">
-        <v>30.03</v>
+        <v>8.41</v>
       </c>
       <c r="F12" s="11" t="n">
-        <v>31.46</v>
+        <v>11.31</v>
       </c>
       <c r="G12" s="11">
         <f>F12-E12</f>
@@ -1086,18 +1112,20 @@
           <t>SMH 10(D-12)</t>
         </is>
       </c>
-      <c r="B13" s="11" t="n"/>
+      <c r="B13" s="11" t="n">
+        <v>8.98</v>
+      </c>
       <c r="C13" s="11" t="n">
-        <v>8.380000000000001</v>
+        <v>7.87</v>
       </c>
       <c r="D13" s="11" t="n">
-        <v>6.57</v>
+        <v>2.63</v>
       </c>
       <c r="E13" s="11" t="n">
-        <v>6.86</v>
+        <v>2.05</v>
       </c>
       <c r="F13" s="11" t="n">
-        <v>7.93</v>
+        <v>4.33</v>
       </c>
       <c r="G13" s="11">
         <f>F13-E13</f>
@@ -1126,7 +1154,9 @@
           <t>SMH 11(D-13)</t>
         </is>
       </c>
-      <c r="B14" s="11" t="n"/>
+      <c r="B14" s="11" t="n">
+        <v>0</v>
+      </c>
       <c r="C14" s="11" t="n">
         <v>0</v>
       </c>
@@ -1166,18 +1196,20 @@
           <t>TOTAl OWE</t>
         </is>
       </c>
-      <c r="B15" s="11" t="n"/>
+      <c r="B15" s="11" t="n">
+        <v>350.79</v>
+      </c>
       <c r="C15" s="11" t="n">
-        <v>318.47</v>
+        <v>298.86</v>
       </c>
       <c r="D15" s="11" t="n">
-        <v>296.55</v>
+        <v>79.69</v>
       </c>
       <c r="E15" s="11" t="n">
-        <v>262.78</v>
+        <v>77.7</v>
       </c>
       <c r="F15" s="11" t="n">
-        <v>290.44</v>
+        <v>102.77</v>
       </c>
       <c r="G15" s="11">
         <f>F15-E15</f>

</xml_diff>